<commit_message>
Actualización RN hasta Step6
</commit_message>
<xml_diff>
--- a/Reglas de Negocio.xlsx
+++ b/Reglas de Negocio.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edgargarcia/Documents/CobranzaEspecializada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A036BC63-090D-6648-BC8B-12507363E4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD185CF6-1174-A241-A76B-2DCDF0314AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-120" windowWidth="38400" windowHeight="20980" activeTab="1" xr2:uid="{6A795986-A781-3842-B5D0-ECE640E20CC7}"/>
+    <workbookView xWindow="-38400" yWindow="120" windowWidth="38400" windowHeight="19380" activeTab="5" xr2:uid="{6A795986-A781-3842-B5D0-ECE640E20CC7}"/>
   </bookViews>
   <sheets>
     <sheet name="SEF STEP 1" sheetId="4" r:id="rId1"/>
     <sheet name="SEF STEP 2" sheetId="1" r:id="rId2"/>
     <sheet name="SEF STEP 3" sheetId="2" r:id="rId3"/>
     <sheet name="SEF STEP 4" sheetId="3" r:id="rId4"/>
+    <sheet name="SEF STEP 5" sheetId="5" r:id="rId5"/>
+    <sheet name="SEF STEP 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="131">
   <si>
     <t>Campo</t>
   </si>
@@ -360,9 +362,6 @@
     <t>COMISIÓN (Cargo)</t>
   </si>
   <si>
-    <t>TRASLADO (Cargo)</t>
-  </si>
-  <si>
     <t>Input, con formato de hasta 7 caracteres numericos. Si es menor a 7, rellenar con CERO a la izquieda</t>
   </si>
   <si>
@@ -379,13 +378,70 @@
   </si>
   <si>
     <t>Multiselect, debe seleccionar al menos 1, hasta 4 opciones</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Perfil</t>
+  </si>
+  <si>
+    <t>Apellido Paterno</t>
+  </si>
+  <si>
+    <t>Apellido Materno</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>Tipo contacto</t>
+  </si>
+  <si>
+    <t>DIFERENCIAS LOCALES</t>
+  </si>
+  <si>
+    <t>REPORTE DE DIFERENCIAS CENTRALIZADO</t>
+  </si>
+  <si>
+    <t>CONTINGENCIA</t>
+  </si>
+  <si>
+    <t>CAPACITACIÓN SEF</t>
+  </si>
+  <si>
+    <t>Extesión</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>Carga Catálogo de Perfiles SEF</t>
+  </si>
+  <si>
+    <t>Input en formato de hasta 8 caracteres alfanumericos</t>
+  </si>
+  <si>
+    <t>Clave usuario</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
+  </si>
+  <si>
+    <t>OBLIGATORIO, cuando Tipo Contrato es SEF ELECTRÓNICO</t>
+  </si>
+  <si>
+    <t>OPCIONAL, cuando Tipo Contrato es SEF ELECTRÓNICO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -413,13 +469,25 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -434,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,6 +536,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,7 +894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF7A3E1-D652-3244-BD4D-DCEC9F0E6CF7}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="143" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -932,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092F2984-364B-734F-B98A-7422D9B8F938}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:F15"/>
+    <sheetView zoomScale="102" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1089,10 +1178,10 @@
         <v>66</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1101,7 +1190,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1111,7 +1200,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1121,12 +1210,12 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1146,9 +1235,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>67</v>
       </c>
@@ -1315,7 +1402,7 @@
         <v>66</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1332,7 +1419,7 @@
         <v>66</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1416,7 +1503,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="F10:F13"/>
     <mergeCell ref="D10:D13"/>
@@ -1445,6 +1532,7 @@
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A14:A15"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="F17:F19"/>
@@ -1459,7 +1547,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1540,64 +1628,64 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="8" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="8" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="8" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="8" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -1618,20 +1706,20 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="1" t="s">
+      <c r="B12" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1799,10 +1887,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD239FD-D757-5B4A-A0F6-B08F8DC94A60}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1843,34 +1931,34 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="B3" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="11" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
@@ -1893,20 +1981,20 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="11" t="s">
+      <c r="B6" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1943,7 +2031,7 @@
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2020,25 +2108,15 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B9:B10"/>
@@ -2051,4 +2129,665 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92DA322-D98C-1C44-A212-7994D31FC4AE}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.1640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="57" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:6" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17"/>
+      <c r="F17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="F3:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA116A0-E817-084E-AC93-05B375A48338}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.1640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="57" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:6" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="F3:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RN Steps 2,3 y 6
</commit_message>
<xml_diff>
--- a/Reglas de Negocio.xlsx
+++ b/Reglas de Negocio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edgargarcia/Documents/CobranzaEspecializada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79F7C3F-94F1-6247-B955-2EB88F0BD0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B430A1-8EBB-7D40-8496-1444A3EF8F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="120" windowWidth="38380" windowHeight="19380" activeTab="2" xr2:uid="{6A795986-A781-3842-B5D0-ECE640E20CC7}"/>
   </bookViews>
@@ -1692,7 +1692,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>